<commit_message>
12 avril : travail sur build agregate from source
</commit_message>
<xml_diff>
--- a/src/countries/france/data/sources/pfam_tous_regimes.xlsx
+++ b/src/countries/france/data/sources/pfam_tous_regimes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="22710" windowHeight="7335"/>
+    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="22710" windowHeight="9450" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="benef" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="sources" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <oleSize ref="A1:Q23"/>
+  <oleSize ref="A1:K20"/>
 </workbook>
 </file>
 
@@ -1059,6 +1059,10 @@
     </xf>
     <xf numFmtId="166" fontId="26" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="26" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="3" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1077,10 +1081,6 @@
     <xf numFmtId="165" fontId="3" fillId="3" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Milliers" xfId="1" builtinId="3"/>
@@ -1442,8 +1442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1833,14 +1833,14 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C16" s="131"/>
-      <c r="D16" s="131"/>
-      <c r="E16" s="131"/>
-      <c r="F16" s="131"/>
-      <c r="G16" s="131"/>
-      <c r="H16" s="131"/>
-      <c r="I16" s="131"/>
-      <c r="J16" s="131"/>
+      <c r="C16" s="125"/>
+      <c r="D16" s="125"/>
+      <c r="E16" s="125"/>
+      <c r="F16" s="125"/>
+      <c r="G16" s="125"/>
+      <c r="H16" s="125"/>
+      <c r="I16" s="125"/>
+      <c r="J16" s="125"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2213,7 +2213,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2246,13 +2246,13 @@
       <c r="N1" s="81"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="124" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="125"/>
-      <c r="C2" s="125"/>
-      <c r="D2" s="125"/>
-      <c r="E2" s="126"/>
+      <c r="A2" s="126" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="127"/>
+      <c r="C2" s="127"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="128"/>
       <c r="F2" s="80"/>
       <c r="G2" s="81"/>
       <c r="H2" s="81"/>
@@ -2510,7 +2510,7 @@
       <c r="J12" s="97">
         <v>51956.804759457642</v>
       </c>
-      <c r="K12" s="130" t="s">
+      <c r="K12" s="124" t="s">
         <v>116</v>
       </c>
     </row>
@@ -2726,28 +2726,28 @@
       <c r="A20" s="82" t="s">
         <v>117</v>
       </c>
-      <c r="B20" s="131">
+      <c r="B20" s="125">
         <v>631080</v>
       </c>
-      <c r="C20" s="131">
+      <c r="C20" s="125">
         <v>649920</v>
       </c>
-      <c r="D20" s="131">
+      <c r="D20" s="125">
         <v>650640</v>
       </c>
-      <c r="E20" s="131">
+      <c r="E20" s="125">
         <v>635400</v>
       </c>
-      <c r="F20" s="131">
+      <c r="F20" s="125">
         <v>629640</v>
       </c>
-      <c r="G20" s="131">
+      <c r="G20" s="125">
         <v>639720</v>
       </c>
-      <c r="H20" s="131">
+      <c r="H20" s="125">
         <v>626640</v>
       </c>
-      <c r="I20" s="131">
+      <c r="I20" s="125">
         <v>623481.65711349167</v>
       </c>
       <c r="J20" s="93"/>
@@ -2772,7 +2772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -2787,13 +2787,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="129" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="128"/>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
-      <c r="E1" s="129"/>
+      <c r="B1" s="130"/>
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="131"/>
       <c r="F1" s="85"/>
       <c r="G1" s="86"/>
       <c r="H1" s="87"/>

</xml_diff>

<commit_message>
commit dev 15 avril
</commit_message>
<xml_diff>
--- a/src/countries/france/data/sources/pfam_tous_regimes.xlsx
+++ b/src/countries/france/data/sources/pfam_tous_regimes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="22710" windowHeight="7335"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="13440" windowHeight="12945" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="benef" sheetId="1" r:id="rId1"/>
@@ -15,12 +15,12 @@
     <sheet name="sources" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <oleSize ref="A1:Q23"/>
+  <oleSize ref="A1:I40"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="118">
   <si>
     <t>Tableau 2 - Bénéficiaires tous régimes France métropolitaine</t>
   </si>
@@ -1059,6 +1059,10 @@
     </xf>
     <xf numFmtId="166" fontId="26" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="26" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="3" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1077,10 +1081,6 @@
     <xf numFmtId="165" fontId="3" fillId="3" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Milliers" xfId="1" builtinId="3"/>
@@ -1440,10 +1440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1483,9 +1483,9 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="103" t="s">
-        <v>94</v>
+        <v>115</v>
       </c>
       <c r="B2" s="96">
         <v>4528000</v>
@@ -1515,23 +1515,23 @@
         <v>4666178.0750013515</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="105" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="103" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="96"/>
+      <c r="C3" s="106"/>
+      <c r="D3" s="106"/>
+      <c r="E3" s="106"/>
+      <c r="F3" s="106"/>
+      <c r="G3" s="106"/>
+      <c r="H3" s="106"/>
+      <c r="I3" s="106"/>
+      <c r="J3" s="106"/>
+    </row>
+    <row r="4" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="103" t="s">
         <v>95</v>
-      </c>
-      <c r="B3" s="98"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="103" t="s">
-        <v>96</v>
       </c>
       <c r="B4" s="98"/>
       <c r="C4" s="97"/>
@@ -1543,304 +1543,318 @@
       <c r="I4" s="97"/>
       <c r="J4" s="97"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="103" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="98"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="97"/>
+      <c r="G5" s="97"/>
+      <c r="H5" s="97"/>
+      <c r="I5" s="97"/>
+      <c r="J5" s="97"/>
+    </row>
+    <row r="6" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="103" t="s">
         <v>97</v>
       </c>
-      <c r="B5" s="96">
+      <c r="B6" s="96">
         <v>880000</v>
       </c>
-      <c r="C5" s="97">
+      <c r="C6" s="97">
         <v>873480</v>
       </c>
-      <c r="D5" s="97">
+      <c r="D6" s="97">
         <v>863030</v>
       </c>
-      <c r="E5" s="97">
+      <c r="E6" s="97">
         <v>844330</v>
       </c>
-      <c r="F5" s="97">
+      <c r="F6" s="97">
         <v>826160</v>
       </c>
-      <c r="G5" s="97">
+      <c r="G6" s="97">
         <v>831690</v>
       </c>
-      <c r="H5" s="97">
+      <c r="H6" s="97">
         <v>831120</v>
       </c>
-      <c r="I5" s="97">
+      <c r="I6" s="97">
         <v>829210</v>
       </c>
-      <c r="J5" s="97">
+      <c r="J6" s="97">
         <v>826390.79801152879</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="103" t="s">
+    <row r="7" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="103" t="s">
         <v>98</v>
       </c>
-      <c r="B6" s="96">
+      <c r="B7" s="96">
         <v>2922000</v>
       </c>
-      <c r="C6" s="97">
+      <c r="C7" s="97">
         <v>2927100</v>
       </c>
-      <c r="D6" s="97">
+      <c r="D7" s="97">
         <v>2900240</v>
       </c>
-      <c r="E6" s="97">
+      <c r="E7" s="97">
         <v>2849520</v>
       </c>
-      <c r="F6" s="97">
+      <c r="F7" s="97">
         <v>2804760</v>
       </c>
-      <c r="G6" s="97">
+      <c r="G7" s="97">
         <v>2903930</v>
       </c>
-      <c r="H6" s="97">
+      <c r="H7" s="97">
         <v>2858690</v>
       </c>
-      <c r="I6" s="97">
+      <c r="I7" s="97">
         <v>2849880</v>
       </c>
-      <c r="J6" s="97">
+      <c r="J7" s="97">
         <v>2816232.2034732876</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="104" t="s">
+    <row r="8" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="104" t="s">
         <v>99</v>
       </c>
-      <c r="B7" s="96">
-        <v>0</v>
-      </c>
-      <c r="C7" s="97">
+      <c r="B8" s="96">
+        <v>0</v>
+      </c>
+      <c r="C8" s="97">
         <v>755990</v>
       </c>
-      <c r="D7" s="97">
+      <c r="D8" s="97">
         <v>1430540</v>
       </c>
-      <c r="E7" s="97">
+      <c r="E8" s="97">
         <v>2022950</v>
       </c>
-      <c r="F7" s="97">
+      <c r="F8" s="97">
         <v>2119830</v>
       </c>
-      <c r="G7" s="97">
+      <c r="G8" s="97">
         <v>2216820</v>
       </c>
-      <c r="H7" s="97">
+      <c r="H8" s="97">
         <v>2269800</v>
       </c>
-      <c r="I7" s="97">
+      <c r="I8" s="97">
         <v>2289036</v>
       </c>
-      <c r="J7" s="97">
+      <c r="J8" s="97">
         <v>2292799.27096391</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="103" t="s">
+    <row r="9" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="103" t="s">
         <v>100</v>
       </c>
-      <c r="B8" s="96">
-        <v>0</v>
-      </c>
-      <c r="C8" s="97">
+      <c r="B9" s="96">
+        <v>0</v>
+      </c>
+      <c r="C9" s="97">
         <v>631080</v>
       </c>
-      <c r="D8" s="97">
+      <c r="D9" s="97">
         <v>649920</v>
       </c>
-      <c r="E8" s="97">
+      <c r="E9" s="97">
         <v>650640</v>
       </c>
-      <c r="F8" s="97">
+      <c r="F9" s="97">
         <v>635400</v>
       </c>
-      <c r="G8" s="97">
+      <c r="G9" s="97">
         <v>629640</v>
       </c>
-      <c r="H8" s="97">
+      <c r="H9" s="97">
         <v>639720</v>
       </c>
-      <c r="I8" s="97">
+      <c r="I9" s="97">
         <v>626640</v>
       </c>
-      <c r="J8" s="97">
+      <c r="J9" s="97">
         <v>623481.65711349167</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="103" t="s">
+    <row r="10" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="103" t="s">
         <v>101</v>
       </c>
-      <c r="B9" s="96">
-        <v>0</v>
-      </c>
-      <c r="C9" s="97">
+      <c r="B10" s="96">
+        <v>0</v>
+      </c>
+      <c r="C10" s="97">
         <v>662350</v>
       </c>
-      <c r="D9" s="97">
+      <c r="D10" s="97">
         <v>1278520</v>
       </c>
-      <c r="E9" s="97">
+      <c r="E10" s="97">
         <v>1814870</v>
       </c>
-      <c r="F9" s="97">
+      <c r="F10" s="97">
         <v>1822430</v>
       </c>
-      <c r="G9" s="97">
+      <c r="G10" s="97">
         <v>1860880</v>
       </c>
-      <c r="H9" s="97">
+      <c r="H10" s="97">
         <v>1856900</v>
       </c>
-      <c r="I9" s="97">
+      <c r="I10" s="97">
         <v>1870070</v>
       </c>
-      <c r="J9" s="97">
+      <c r="J10" s="97">
         <v>1859913.7298134691</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="103" t="s">
+    <row r="11" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="103" t="s">
         <v>102</v>
       </c>
-      <c r="B10" s="96">
-        <v>0</v>
-      </c>
-      <c r="C10" s="97">
+      <c r="B11" s="96">
+        <v>0</v>
+      </c>
+      <c r="C11" s="97">
         <v>183710</v>
       </c>
-      <c r="D10" s="97">
+      <c r="D11" s="97">
         <v>408820</v>
       </c>
-      <c r="E10" s="97">
+      <c r="E11" s="97">
         <v>601760</v>
       </c>
-      <c r="F10" s="97">
+      <c r="F11" s="97">
         <v>592780</v>
       </c>
-      <c r="G10" s="97">
+      <c r="G11" s="97">
         <v>580310</v>
       </c>
-      <c r="H10" s="97">
+      <c r="H11" s="97">
         <v>565880</v>
       </c>
-      <c r="I10" s="97">
+      <c r="I11" s="97">
         <v>548760</v>
       </c>
-      <c r="J10" s="97">
+      <c r="J11" s="97">
         <v>533584.98695263092</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="103" t="s">
+    <row r="12" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="103" t="s">
         <v>103</v>
       </c>
-      <c r="B11" s="96">
-        <v>0</v>
-      </c>
-      <c r="C11" s="97">
-        <v>0</v>
-      </c>
-      <c r="D11" s="97">
-        <v>0</v>
-      </c>
-      <c r="E11" s="97">
+      <c r="B12" s="96">
+        <v>0</v>
+      </c>
+      <c r="C12" s="97">
+        <v>0</v>
+      </c>
+      <c r="D12" s="97">
+        <v>0</v>
+      </c>
+      <c r="E12" s="97">
         <v>680</v>
       </c>
-      <c r="F11" s="97">
+      <c r="F12" s="97">
         <v>2300</v>
       </c>
-      <c r="G11" s="97">
+      <c r="G12" s="97">
         <v>2100</v>
       </c>
-      <c r="H11" s="97">
+      <c r="H12" s="97">
         <v>2230</v>
       </c>
-      <c r="I11" s="97">
+      <c r="I12" s="97">
         <v>2250</v>
       </c>
-      <c r="J11" s="97">
+      <c r="J12" s="97">
         <v>2377.7472527472523</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="103" t="s">
+    <row r="13" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="103" t="s">
         <v>104</v>
       </c>
-      <c r="B12" s="96">
-        <v>0</v>
-      </c>
-      <c r="C12" s="97">
+      <c r="B13" s="96">
+        <v>0</v>
+      </c>
+      <c r="C13" s="97">
         <v>111320</v>
       </c>
-      <c r="D12" s="97">
+      <c r="D13" s="97">
         <v>315700</v>
       </c>
-      <c r="E12" s="97">
+      <c r="E13" s="97">
         <v>528000</v>
       </c>
-      <c r="F12" s="97">
+      <c r="F13" s="97">
         <v>634970</v>
       </c>
-      <c r="G12" s="97">
+      <c r="G13" s="97">
         <v>725620</v>
       </c>
-      <c r="H12" s="97">
+      <c r="H13" s="97">
         <v>799030</v>
       </c>
-      <c r="I12" s="97">
+      <c r="I13" s="97">
         <v>828420</v>
       </c>
-      <c r="J12" s="97">
+      <c r="J13" s="97">
         <v>860051.56998945796</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="103" t="s">
+    <row r="14" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="103" t="s">
         <v>105</v>
       </c>
-      <c r="B13" s="96">
+      <c r="B14" s="96">
         <v>586000</v>
       </c>
-      <c r="C13" s="97">
+      <c r="C14" s="97">
         <v>597100</v>
       </c>
-      <c r="D13" s="97">
+      <c r="D14" s="97">
         <v>604250</v>
       </c>
-      <c r="E13" s="97">
+      <c r="E14" s="97">
         <v>605660</v>
       </c>
-      <c r="F13" s="97">
+      <c r="F14" s="97">
         <v>628320</v>
       </c>
-      <c r="G13" s="97">
+      <c r="G14" s="97">
         <v>621060</v>
       </c>
-      <c r="H13" s="97">
+      <c r="H14" s="97">
         <v>651090</v>
       </c>
-      <c r="I13" s="97">
+      <c r="I14" s="97">
         <v>647230</v>
       </c>
-      <c r="J13" s="97">
+      <c r="J14" s="97">
         <v>642776.17620313715</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C16" s="131"/>
-      <c r="D16" s="131"/>
-      <c r="E16" s="131"/>
-      <c r="F16" s="131"/>
-      <c r="G16" s="131"/>
-      <c r="H16" s="131"/>
-      <c r="I16" s="131"/>
-      <c r="J16" s="131"/>
+    <row r="16" spans="1:10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="125"/>
+      <c r="D17" s="125"/>
+      <c r="E17" s="125"/>
+      <c r="F17" s="125"/>
+      <c r="G17" s="125"/>
+      <c r="H17" s="125"/>
+      <c r="I17" s="125"/>
+      <c r="J17" s="125"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1849,10 +1863,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1897,7 +1911,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="103" t="s">
         <v>115</v>
       </c>
@@ -1926,282 +1940,312 @@
         <v>11822000000</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="105" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="103" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="121"/>
+      <c r="C3" s="122"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="106"/>
+      <c r="F3" s="106"/>
+      <c r="G3" s="106"/>
+      <c r="H3" s="122"/>
+      <c r="I3" s="122"/>
+    </row>
+    <row r="4" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="103" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="98"/>
-      <c r="C3" s="106"/>
-      <c r="D3" s="108"/>
-      <c r="E3" s="106">
+      <c r="B4" s="98"/>
+      <c r="C4" s="106"/>
+      <c r="D4" s="108"/>
+      <c r="E4" s="106">
         <v>109020000</v>
       </c>
-      <c r="F3" s="106">
+      <c r="F4" s="106">
         <v>104850000</v>
       </c>
-      <c r="G3" s="106">
+      <c r="G4" s="106">
         <v>95470000</v>
       </c>
-      <c r="H3" s="106"/>
-      <c r="I3" s="106"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="103" t="s">
+      <c r="H4" s="106"/>
+      <c r="I4" s="106"/>
+    </row>
+    <row r="5" spans="1:9" s="105" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="103" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="98"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="108"/>
+      <c r="E5" s="106"/>
+      <c r="F5" s="106"/>
+      <c r="G5" s="106"/>
+      <c r="H5" s="106"/>
+      <c r="I5" s="106"/>
+    </row>
+    <row r="6" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="103" t="s">
         <v>97</v>
       </c>
-      <c r="B4" s="96">
+      <c r="B6" s="96">
         <v>1521900000</v>
       </c>
-      <c r="C4" s="106">
+      <c r="C6" s="106">
         <v>1537900000</v>
       </c>
-      <c r="D4" s="108">
+      <c r="D6" s="108">
         <v>1557400000</v>
       </c>
-      <c r="E4" s="106">
+      <c r="E6" s="106">
         <v>1559800000</v>
       </c>
-      <c r="F4" s="106">
+      <c r="F6" s="106">
         <v>1549200000</v>
       </c>
-      <c r="G4" s="106">
+      <c r="G6" s="106">
         <v>1558200000</v>
       </c>
-      <c r="H4" s="106">
+      <c r="H6" s="106">
         <v>1591500000</v>
       </c>
-      <c r="I4" s="106">
+      <c r="I6" s="106">
         <v>1593800000</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="103" t="s">
+    <row r="7" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="103" t="s">
         <v>98</v>
       </c>
-      <c r="B5" s="96">
+      <c r="B7" s="96">
         <v>1266800000</v>
       </c>
-      <c r="C5" s="106">
+      <c r="C7" s="106">
         <v>1295000000</v>
       </c>
-      <c r="D5" s="108">
+      <c r="D7" s="108">
         <v>1304000000</v>
       </c>
-      <c r="E5" s="106">
+      <c r="E7" s="106">
         <v>1312000000</v>
       </c>
-      <c r="F5" s="106">
+      <c r="F7" s="106">
         <v>1304400000</v>
       </c>
-      <c r="G5" s="106">
+      <c r="G7" s="106">
         <v>1404900000</v>
       </c>
-      <c r="H5" s="106">
+      <c r="H7" s="106">
         <v>1412000000</v>
       </c>
-      <c r="I5" s="106">
+      <c r="I7" s="106">
         <v>1406000000</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="104" t="s">
+    <row r="8" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="104" t="s">
         <v>99</v>
       </c>
-      <c r="B6" s="96">
-        <v>0</v>
-      </c>
-      <c r="C6" s="106">
+      <c r="B8" s="96">
+        <v>0</v>
+      </c>
+      <c r="C8" s="106">
         <v>1751200000</v>
       </c>
-      <c r="D6" s="108">
+      <c r="D8" s="108">
         <v>5092100000</v>
       </c>
-      <c r="E6" s="106">
+      <c r="E8" s="106">
         <v>8604600000</v>
       </c>
-      <c r="F6" s="106">
+      <c r="F8" s="106">
         <v>10345300000</v>
       </c>
-      <c r="G6" s="106">
+      <c r="G8" s="106">
         <v>11166000000</v>
       </c>
-      <c r="H6" s="106">
+      <c r="H8" s="106">
         <v>11791700000</v>
       </c>
-      <c r="I6" s="106">
+      <c r="I8" s="106">
         <v>12119200000</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="103" t="s">
+    <row r="9" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="103" t="s">
         <v>100</v>
       </c>
-      <c r="B7" s="96">
-        <v>0</v>
-      </c>
-      <c r="C7" s="106">
+      <c r="B9" s="96">
+        <v>0</v>
+      </c>
+      <c r="C9" s="106">
         <v>563200000</v>
       </c>
-      <c r="D7" s="108">
+      <c r="D9" s="108">
         <v>567700000</v>
       </c>
-      <c r="E7" s="106">
+      <c r="E9" s="106">
         <v>595800000</v>
       </c>
-      <c r="F7" s="106">
+      <c r="F9" s="106">
         <v>595600000</v>
       </c>
-      <c r="G7" s="106">
+      <c r="G9" s="106">
         <v>613700000</v>
       </c>
-      <c r="H7" s="106">
+      <c r="H9" s="106">
         <v>630000000</v>
       </c>
-      <c r="I7" s="106">
+      <c r="I9" s="106">
         <v>634000000</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="103" t="s">
+    <row r="10" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="103" t="s">
         <v>101</v>
       </c>
-      <c r="B8" s="96">
-        <v>0</v>
-      </c>
-      <c r="C8" s="106">
+      <c r="B10" s="96">
+        <v>0</v>
+      </c>
+      <c r="C10" s="106">
         <v>724200000</v>
       </c>
-      <c r="D8" s="108">
+      <c r="D10" s="108">
         <v>2051900000</v>
       </c>
-      <c r="E8" s="106">
+      <c r="E10" s="106">
         <v>3306600000</v>
       </c>
-      <c r="F8" s="106">
+      <c r="F10" s="106">
         <v>3841600000</v>
       </c>
-      <c r="G8" s="106">
+      <c r="G10" s="106">
         <v>3947700000</v>
       </c>
-      <c r="H8" s="106">
+      <c r="H10" s="106">
         <v>4066500000</v>
       </c>
-      <c r="I8" s="106">
+      <c r="I10" s="106">
         <v>4080500000</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="103" t="s">
+    <row r="11" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="103" t="s">
         <v>102</v>
       </c>
-      <c r="B9" s="96">
-        <v>0</v>
-      </c>
-      <c r="C9" s="106">
+      <c r="B11" s="96">
+        <v>0</v>
+      </c>
+      <c r="C11" s="106">
         <v>285800000</v>
       </c>
-      <c r="D9" s="108">
+      <c r="D11" s="108">
         <v>1150700000</v>
       </c>
-      <c r="E9" s="106">
+      <c r="E11" s="106">
         <v>1941100000.0000002</v>
       </c>
-      <c r="F9" s="106">
+      <c r="F11" s="106">
         <v>2243400000</v>
       </c>
-      <c r="G9" s="106">
+      <c r="G11" s="106">
         <v>2218200000</v>
       </c>
-      <c r="H9" s="106">
+      <c r="H11" s="106">
         <v>2221600000</v>
       </c>
-      <c r="I9" s="106">
+      <c r="I11" s="106">
         <v>2141800000.0000002</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="103" t="s">
+    <row r="12" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="103" t="s">
         <v>103</v>
       </c>
-      <c r="B10" s="96">
-        <v>0</v>
-      </c>
-      <c r="C10" s="106">
-        <v>0</v>
-      </c>
-      <c r="D10" s="108">
-        <v>0</v>
-      </c>
-      <c r="E10" s="106">
+      <c r="B12" s="96">
+        <v>0</v>
+      </c>
+      <c r="C12" s="106">
+        <v>0</v>
+      </c>
+      <c r="D12" s="108">
+        <v>0</v>
+      </c>
+      <c r="E12" s="106">
         <v>1000000</v>
       </c>
-      <c r="F10" s="106">
+      <c r="F12" s="106">
         <v>17000000</v>
       </c>
-      <c r="G10" s="106"/>
-      <c r="H10" s="106"/>
-      <c r="I10" s="106"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="103" t="s">
+      <c r="G12" s="106"/>
+      <c r="H12" s="106"/>
+      <c r="I12" s="106"/>
+    </row>
+    <row r="13" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="103" t="s">
         <v>104</v>
       </c>
-      <c r="B11" s="96">
-        <v>0</v>
-      </c>
-      <c r="C11" s="106">
+      <c r="B13" s="96">
+        <v>0</v>
+      </c>
+      <c r="C13" s="106">
         <v>178000000</v>
       </c>
-      <c r="D11" s="108">
+      <c r="D13" s="108">
         <v>1321800000</v>
       </c>
-      <c r="E11" s="106">
+      <c r="E13" s="106">
         <v>2760300000</v>
       </c>
-      <c r="F11" s="106">
+      <c r="F13" s="106">
         <v>3648200000</v>
       </c>
-      <c r="G11" s="106">
+      <c r="G13" s="106">
         <v>4386400000</v>
       </c>
-      <c r="H11" s="106">
+      <c r="H13" s="106">
         <v>4873600000</v>
       </c>
-      <c r="I11" s="106">
+      <c r="I13" s="106">
         <v>5262900000</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="103" t="s">
+    <row r="14" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="103" t="s">
         <v>105</v>
       </c>
-      <c r="B12" s="96">
+      <c r="B14" s="96">
         <v>856700000</v>
       </c>
-      <c r="C12" s="107">
+      <c r="C14" s="107">
         <v>887700000</v>
       </c>
-      <c r="D12" s="108">
+      <c r="D14" s="108">
         <v>921200000</v>
       </c>
-      <c r="E12" s="106">
+      <c r="E14" s="106">
         <v>944600000</v>
       </c>
-      <c r="F12" s="106">
+      <c r="F14" s="106">
         <v>1013400000</v>
       </c>
-      <c r="G12" s="106">
+      <c r="G14" s="106">
         <v>1002700000</v>
       </c>
-      <c r="H12" s="106">
+      <c r="H14" s="106">
         <v>1080800000</v>
       </c>
-      <c r="I12" s="106">
+      <c r="I14" s="106">
         <v>1077900000</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="105"/>
+    </row>
+    <row r="18" spans="1:9" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="105"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2246,13 +2290,13 @@
       <c r="N1" s="81"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="124" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="125"/>
-      <c r="C2" s="125"/>
-      <c r="D2" s="125"/>
-      <c r="E2" s="126"/>
+      <c r="A2" s="126" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="127"/>
+      <c r="C2" s="127"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="128"/>
       <c r="F2" s="80"/>
       <c r="G2" s="81"/>
       <c r="H2" s="81"/>
@@ -2510,7 +2554,7 @@
       <c r="J12" s="97">
         <v>51956.804759457642</v>
       </c>
-      <c r="K12" s="130" t="s">
+      <c r="K12" s="124" t="s">
         <v>116</v>
       </c>
     </row>
@@ -2726,28 +2770,28 @@
       <c r="A20" s="82" t="s">
         <v>117</v>
       </c>
-      <c r="B20" s="131">
+      <c r="B20" s="125">
         <v>631080</v>
       </c>
-      <c r="C20" s="131">
+      <c r="C20" s="125">
         <v>649920</v>
       </c>
-      <c r="D20" s="131">
+      <c r="D20" s="125">
         <v>650640</v>
       </c>
-      <c r="E20" s="131">
+      <c r="E20" s="125">
         <v>635400</v>
       </c>
-      <c r="F20" s="131">
+      <c r="F20" s="125">
         <v>629640</v>
       </c>
-      <c r="G20" s="131">
+      <c r="G20" s="125">
         <v>639720</v>
       </c>
-      <c r="H20" s="131">
+      <c r="H20" s="125">
         <v>626640</v>
       </c>
-      <c r="I20" s="131">
+      <c r="I20" s="125">
         <v>623481.65711349167</v>
       </c>
       <c r="J20" s="93"/>
@@ -2787,13 +2831,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="129" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="128"/>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
-      <c r="E1" s="129"/>
+      <c r="B1" s="130"/>
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="131"/>
       <c r="F1" s="85"/>
       <c r="G1" s="86"/>
       <c r="H1" s="87"/>

</xml_diff>